<commit_message>
apresentar tabela com validação de perfil
ajustando para apresentar a tabela com validação do perfil
</commit_message>
<xml_diff>
--- a/banco/tb_armazenamento_ar.xlsx
+++ b/banco/tb_armazenamento_ar.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>numero_caixa</t>
   </si>
@@ -71,15 +71,9 @@
     <t>data_conferencia</t>
   </si>
   <si>
-    <t>gerar_etiqueta</t>
-  </si>
-  <si>
     <t>numero_etiqueta</t>
   </si>
   <si>
-    <t>data_carta_gerada</t>
-  </si>
-  <si>
     <t>ACD</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>SE/BSB</t>
   </si>
   <si>
-    <t>NÃO</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
@@ -134,7 +125,13 @@
     <t>quebra_sequencia</t>
   </si>
   <si>
-    <t>solicitar_correcao</t>
+    <t>NAO</t>
+  </si>
+  <si>
+    <t>corrigido</t>
+  </si>
+  <si>
+    <t>retida</t>
   </si>
 </sst>
 </file>
@@ -453,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,14 +473,12 @@
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,19 +528,16 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>45453</v>
       </c>
@@ -553,7 +545,7 @@
         <v>45840</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>26725386</v>
@@ -574,27 +566,30 @@
         <v>254</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1">
         <v>46051</v>
       </c>
       <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
       <c r="O2" s="1"/>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>45301</v>
       </c>
@@ -602,7 +597,7 @@
         <v>45840</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>26724700</v>
@@ -623,27 +618,30 @@
         <v>1235</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1">
         <v>46051</v>
       </c>
       <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
       <c r="O3" s="1"/>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>45331</v>
       </c>
@@ -651,7 +649,7 @@
         <v>45840</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>26724739</v>
@@ -672,27 +670,30 @@
         <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K4" s="1">
         <v>46051</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>49075</v>
       </c>
@@ -700,7 +701,7 @@
         <v>45840</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>26780425</v>
@@ -721,27 +722,30 @@
         <v>2902</v>
       </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K5" s="1">
         <v>46053</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O5" s="1"/>
-      <c r="P5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="R5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>49768</v>
       </c>
@@ -749,7 +753,7 @@
         <v>45840</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>26788321</v>
@@ -770,27 +774,30 @@
         <v>2773</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K6" s="1">
         <v>46053</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>45967</v>
       </c>
@@ -798,7 +805,7 @@
         <v>45840</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>26736416</v>
@@ -819,25 +826,28 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K7" s="1">
         <v>46051</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" t="s">
-        <v>23</v>
-      </c>
-      <c r="R7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>